<commit_message>
feat: add import user
</commit_message>
<xml_diff>
--- a/public/files/保安公司导入模板.xlsx
+++ b/public/files/保安公司导入模板.xlsx
@@ -64,14 +64,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -104,6 +104,13 @@
       <color rgb="FFFFFFFF"/>
       <name val="宋体-简"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -617,153 +624,153 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -792,6 +799,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1143,13 +1153,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="3" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="32.3653846153846" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.1826923076923" style="2" customWidth="1"/>
@@ -1202,6 +1212,9 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7" spans="3:3">
+      <c r="C7" s="10"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>

</xml_diff>